<commit_message>
retirar os efeitos de cursor do mouse
</commit_message>
<xml_diff>
--- a/backlog-projeto-individual.xlsx
+++ b/backlog-projeto-individual.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\OneDrive - SPTech School\projeto-individual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/nicolas_sampaio_sptech_school/Documents/projeto-individual/Gatices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C72DF27-D3FB-4C90-B7A9-26AB464B0FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{515E67F7-29E9-4035-B711-670DFD54677D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{2AF606DE-C3BC-448B-8EBD-34B42A3F581A}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Burndown" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="181">
   <si>
     <t xml:space="preserve">Requisito </t>
   </si>
@@ -48,12 +49,6 @@
     <t>Classificação</t>
   </si>
   <si>
-    <t>Definir papeis</t>
-  </si>
-  <si>
-    <t>Definir os papéis e responsabilidades de cada membro da equipe</t>
-  </si>
-  <si>
     <t>Essencial</t>
   </si>
   <si>
@@ -66,9 +61,6 @@
     <t>Criar repositório no GitHub</t>
   </si>
   <si>
-    <t>Criar um novo repositório no GitHub para o projeto, garantindo que esteja privado ou público conforme a necessidade</t>
-  </si>
-  <si>
     <t>Documentação atualizada do projeto</t>
   </si>
   <si>
@@ -78,87 +70,42 @@
     <t>Importante</t>
   </si>
   <si>
-    <t>Pesquisar e reunir dados sobre o contexto do negócio</t>
-  </si>
-  <si>
-    <t>Coletar informações relevantes sobre o setor, mercado, e os desafios enfrentados pelo negócio que justificam o projeto.</t>
-  </si>
-  <si>
     <t>Planilha de riscos do projeto</t>
   </si>
   <si>
-    <t>Escrever a seção de justificativa do projeto</t>
-  </si>
-  <si>
-    <t>Detalhar por que o projeto é necessário, incluindo benefícios esperados e alinhamento com os objetivos estratégicos do negócio.</t>
-  </si>
-  <si>
     <t>Especificação da Dashboard</t>
   </si>
   <si>
     <t>Definir o layout e o conteudo que será mostrado na dashboard na dashboard.</t>
   </si>
   <si>
-    <t>Elaborar o escopo do projeto</t>
-  </si>
-  <si>
-    <t>Definir e documentar o escopo do projeto, detalhando o que está dentro e fora do projeto.</t>
-  </si>
-  <si>
     <t>Site estático institucional</t>
   </si>
   <si>
     <t>Execução do protótipo feito no figma, para a criação do site institucional.</t>
   </si>
   <si>
-    <t>Criar o diagrama da visão de negócio</t>
-  </si>
-  <si>
-    <t>Utilizar ferramentas de diagramação para criar um diagrama visual que represente a visão do negócio.</t>
-  </si>
-  <si>
     <t>Site estático dashboard</t>
   </si>
   <si>
     <t>Aplicação da dashboard ao site institucional</t>
   </si>
   <si>
-    <t>Definir o layout e navegação principal do site</t>
-  </si>
-  <si>
-    <t>Planejar a estrutura e navegação do site, determinando a disposição dos elementos principais e a hierarquia de informações.</t>
-  </si>
-  <si>
     <t>Site estático cadastro e login - Prototipo</t>
   </si>
   <si>
     <t>Prototipação da pagina de cadastro e tambem da pagina de login</t>
   </si>
   <si>
-    <t>Desenvolver o menu de navegação</t>
-  </si>
-  <si>
-    <t>Criar o menu que permitirá a navegação entre as principais páginas do site (Início, Quem Somos, Sobre Nós, Contato). focando em usabilidade e clareza</t>
-  </si>
-  <si>
     <t xml:space="preserve">Site estático cadastro e login </t>
   </si>
   <si>
     <t>Aplicar a prototipação ao site institucional.</t>
   </si>
   <si>
-    <t>Desenvolver a página Início</t>
-  </si>
-  <si>
-    <t>Criar a página inicial do site, incluindo o design e o conteúdo relevante para a apresentação da instituição. focando em usabilidade e clareza</t>
-  </si>
-  <si>
     <t>Diagrama de solução</t>
   </si>
   <si>
-    <t>Desenvolver a página Quem Somos</t>
-  </si>
-  <si>
     <t>Criar a página que apresenta a equipe ou a história da instituição, com foco em quem são os responsáveis e os valores da empresa. focando em usabilidade e clareza</t>
   </si>
   <si>
@@ -168,21 +115,12 @@
     <t>Montagens dos entregáveis da sprint 02 na ferramenta de gestão Trello</t>
   </si>
   <si>
-    <t>Desenvolver a página Sobre Nós</t>
-  </si>
-  <si>
-    <t>Criar a página com informações detalhadas sobre a instituição, incluindo missão, visão, e história. focando em usabilidade e clareza</t>
-  </si>
-  <si>
     <t>BacklLog da sprint</t>
   </si>
   <si>
     <t>Montagem do backlog da sprint 02 com os entregáveis que serão solcitados e aplicação a ferramenta de gestão</t>
   </si>
   <si>
-    <t>Desenvolver a página Contato</t>
-  </si>
-  <si>
     <t>Criar a página que inclui um formulário de contato, informações de endereço, telefone e email da instituição. focando em usabilidade e clareza</t>
   </si>
   <si>
@@ -192,9 +130,6 @@
     <t>Modelagem lógica do banco de dados para aplicação do projeto</t>
   </si>
   <si>
-    <t>Definir os requisitos funcionais do simulador financeiro</t>
-  </si>
-  <si>
     <t>Especificar as funcionalidades que o simulador deve ter, como cálculos financeiros, entradas e saídas de dados, e interação do usuário.</t>
   </si>
   <si>
@@ -207,9 +142,6 @@
     <t>Tabelas criadas em BD local</t>
   </si>
   <si>
-    <t>Desenvolva os cálculos financeiros</t>
-  </si>
-  <si>
     <t>Programar as operações de cálculo financeiro baseadas nos dados de entrada do usuário.</t>
   </si>
   <si>
@@ -586,6 +518,69 @@
   </si>
   <si>
     <t xml:space="preserve">Grupo 11 - WineGuard - BackLog </t>
+  </si>
+  <si>
+    <t>Documentação do Projeto</t>
+  </si>
+  <si>
+    <t>Organizar a ferramenta de gestão</t>
+  </si>
+  <si>
+    <t>Criar um nome e logo para o site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definir a palleta de cores para o site </t>
+  </si>
+  <si>
+    <t>Desenvolver a página Curiosidades</t>
+  </si>
+  <si>
+    <t>Desenvolver a página Sobre</t>
+  </si>
+  <si>
+    <t>Desenvolver a página de Criação de pet</t>
+  </si>
+  <si>
+    <t>Desenvolver o rodapé do site</t>
+  </si>
+  <si>
+    <t>Desenvolver a página de login do site</t>
+  </si>
+  <si>
+    <t>Desenvoler a página de cadastro do site</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fazer a documentação completa do projeto</t>
+  </si>
+  <si>
+    <t>Criação do repositório para versionamento do projeto</t>
+  </si>
+  <si>
+    <t>Organizar o backlog e os requistos na ferramenta de gestão Trello</t>
+  </si>
+  <si>
+    <t>Definir as cores para identidade visual do projeto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criação da logo do site </t>
+  </si>
+  <si>
+    <t>Desenvolver o cabeçalho com barra de navegação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento do header e da navbar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolver a página de Início </t>
+  </si>
+  <si>
+    <t>Planejar e desenvolver a disposição dos elementos da página de início</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criar a página que apresenta algumas curiosidades sobre gatos </t>
+  </si>
+  <si>
+    <t>Criar a página em que o usuário terá a possibilidade de criar um gato virtual</t>
   </si>
 </sst>
 </file>
@@ -891,7 +886,15 @@
     <cellStyle name="Ênfase6" xfId="1" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="34">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8ED973"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -994,6 +997,30 @@
       <fill>
         <patternFill>
           <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8ED973"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8ED973"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8ED973"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1196,14 +1223,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8ED973"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border outline="0">
@@ -4406,21 +4425,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2100501B-8E1F-4228-9C83-8B1543D6389D}" name="Tabela2" displayName="Tabela2" ref="B3:J76" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" tableBorderDxfId="28">
-  <autoFilter ref="B3:J76" xr:uid="{2100501B-8E1F-4228-9C83-8B1543D6389D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:D38">
-    <sortCondition sortBy="cellColor" ref="D3:D38" dxfId="27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2100501B-8E1F-4228-9C83-8B1543D6389D}" name="Tabela2" displayName="Tabela2" ref="B3:J75" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" tableBorderDxfId="31">
+  <autoFilter ref="B3:J75" xr:uid="{2100501B-8E1F-4228-9C83-8B1543D6389D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:D37">
+    <sortCondition sortBy="cellColor" ref="D3:D37" dxfId="17"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{BEF3E0F9-664B-4131-9E32-84C2DF122F1B}" name="Requisito " dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{D9C38E4B-F210-4D7A-B114-A20A6E2BAB88}" name="Descrição" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{B682C8CE-E476-40AE-B768-E19EC4A05A63}" name="Classificação" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{FCD4E3F4-7FC2-4C3C-A571-52A27DB44A73}" name="Tamanho" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{3503DCC4-B051-4B4B-A453-26FA852E7850}" name="Fibonacci" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{4F91D122-B58A-488D-8C91-9C7AAD7F5257}" name="Sprint" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{ABA96F96-0509-4C34-B2F8-D5F5BDD50256}" name="Responsável" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{DB455FF8-F0C8-4361-9AF3-749A507C9FD8}" name="Prioridade" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{27352BDF-13DF-4FB0-8222-06F89A53A901}" name="Status" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{BEF3E0F9-664B-4131-9E32-84C2DF122F1B}" name="Requisito " dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{D9C38E4B-F210-4D7A-B114-A20A6E2BAB88}" name="Descrição" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{B682C8CE-E476-40AE-B768-E19EC4A05A63}" name="Classificação" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{FCD4E3F4-7FC2-4C3C-A571-52A27DB44A73}" name="Tamanho" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{3503DCC4-B051-4B4B-A453-26FA852E7850}" name="Fibonacci" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{4F91D122-B58A-488D-8C91-9C7AAD7F5257}" name="Sprint" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{ABA96F96-0509-4C34-B2F8-D5F5BDD50256}" name="Responsável" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{DB455FF8-F0C8-4361-9AF3-749A507C9FD8}" name="Prioridade" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{27352BDF-13DF-4FB0-8222-06F89A53A901}" name="Status" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4430,7 +4449,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4930C89A-2589-4117-AFBE-C17347021361}" name="Tabela3" displayName="Tabela3" ref="B3:D9" totalsRowShown="0">
   <autoFilter ref="B3:D9" xr:uid="{4930C89A-2589-4117-AFBE-C17347021361}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{DA276916-4CB6-4E6B-8B09-80EB1024C623}" name="Data" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{DA276916-4CB6-4E6B-8B09-80EB1024C623}" name="Data" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{D9AC9207-339D-4DA9-9DC6-78939AEC1350}" name="Planejamento fibonacci"/>
     <tableColumn id="3" xr3:uid="{694CA19D-0A10-409A-B552-CC3FF84D9A7B}" name="Realizado"/>
   </tableColumns>
@@ -4442,7 +4461,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{04E4E8AD-6331-47FE-A262-355F7FBD434C}" name="Tabela35" displayName="Tabela35" ref="I3:K10" totalsRowShown="0">
   <autoFilter ref="I3:K10" xr:uid="{04E4E8AD-6331-47FE-A262-355F7FBD434C}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E7876DF8-0A4D-488C-A914-EB019DB131C5}" name="Data" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{E7876DF8-0A4D-488C-A914-EB019DB131C5}" name="Data" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{85A6F1FC-F9A6-4D32-92C1-D1A6995B8145}" name="Planejamento fibonacci"/>
     <tableColumn id="3" xr3:uid="{23E60C6D-1CB6-473A-AD51-28129329C065}" name="Realizado"/>
   </tableColumns>
@@ -4454,7 +4473,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1E29810C-7BBD-40AE-9435-3ABC7BA52629}" name="Tabela356" displayName="Tabela356" ref="P3:R8" totalsRowShown="0">
   <autoFilter ref="P3:R8" xr:uid="{1E29810C-7BBD-40AE-9435-3ABC7BA52629}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C2FE972F-14DE-4CD3-B70D-A33B41FB1263}" name="Data" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{C2FE972F-14DE-4CD3-B70D-A33B41FB1263}" name="Data" dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{2FE94DB3-910A-4273-A272-087E2FC673A3}" name="Planejamento fibonacci"/>
     <tableColumn id="3" xr3:uid="{2674E050-3836-4B62-8FBF-B6B39498F01E}" name="Realizado"/>
   </tableColumns>
@@ -4781,8 +4800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC7B248-B611-44D6-BE4C-6F9175744526}">
   <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4801,7 +4820,7 @@
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="22" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -4823,1183 +4842,1183 @@
         <v>2</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>5</v>
-      </c>
       <c r="E4" s="16" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="F4" s="16">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I4" s="16">
         <v>1</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>9</v>
+        <v>171</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="F5" s="16">
         <v>3</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="I5" s="16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J5" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
-        <v>13</v>
+        <v>161</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>14</v>
+        <v>172</v>
       </c>
       <c r="D6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" s="16">
         <v>5</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="F6" s="16">
-        <v>21</v>
-      </c>
       <c r="G6" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="I6" s="16">
         <v>1</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
-        <v>16</v>
+        <v>163</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="F7" s="16">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="I7" s="16">
         <v>1</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
-        <v>20</v>
+        <v>162</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>21</v>
+        <v>174</v>
       </c>
       <c r="D8" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="16">
         <v>5</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="F8" s="16">
-        <v>8</v>
-      </c>
       <c r="G8" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I8" s="16">
         <v>1</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
-        <v>24</v>
+        <v>175</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>25</v>
+        <v>176</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="F9" s="16">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="I9" s="16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>29</v>
+        <v>178</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="F10" s="16">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I10" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
-        <v>32</v>
+        <v>165</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="F11" s="16">
         <v>8</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="I11" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
-        <v>36</v>
+        <v>164</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>37</v>
+        <v>179</v>
       </c>
       <c r="D12" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="16">
         <v>5</v>
       </c>
-      <c r="E12" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="F12" s="16">
-        <v>13</v>
-      </c>
       <c r="G12" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="I12" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
-        <v>39</v>
+        <v>166</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>40</v>
+        <v>180</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="F13" s="16">
         <v>5</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="I13" s="16">
         <v>3</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
-        <v>43</v>
+        <v>167</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="F14" s="16">
         <v>5</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="I14" s="16">
         <v>3</v>
       </c>
       <c r="J14" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="16" t="s">
-        <v>47</v>
+        <v>168</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="F15" s="16">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="I15" s="16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J15" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="16" t="s">
-        <v>51</v>
+        <v>169</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="F16" s="16">
         <v>21</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="I16" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J16" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="16" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="F17" s="16">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="I17" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="16" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D18" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="16">
         <v>5</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="F18" s="16">
-        <v>13</v>
-      </c>
       <c r="G18" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="I18" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="16" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="F19" s="16">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="I19" s="16">
         <v>2</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="16" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="F20" s="16">
         <v>8</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="I20" s="16">
         <v>2</v>
       </c>
       <c r="J20" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="16" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D21" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="16">
         <v>5</v>
       </c>
-      <c r="E21" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="F21" s="16">
-        <v>8</v>
-      </c>
       <c r="G21" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="I21" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="16" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="F22" s="16">
         <v>5</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="I22" s="16">
         <v>1</v>
       </c>
       <c r="J22" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>76</v>
+        <v>54</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>55</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="F23" s="16">
         <v>5</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="I23" s="16">
         <v>1</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>78</v>
+        <v>57</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>58</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="F24" s="16">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="I24" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J24" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="16" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="F25" s="16">
         <v>8</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="I25" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="16" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="F26" s="16">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="I26" s="16">
         <v>1</v>
       </c>
       <c r="J26" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="16" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="F27" s="16">
         <v>3</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="I27" s="16">
         <v>1</v>
       </c>
       <c r="J27" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="16" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>79</v>
+        <v>9</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="F28" s="16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="I28" s="16">
         <v>1</v>
       </c>
       <c r="J28" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="16" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="F29" s="16">
         <v>5</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="I29" s="16">
         <v>1</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="16" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="F30" s="16">
         <v>5</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H30" s="18" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="I30" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J30" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="16" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="F31" s="16">
         <v>5</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="I31" s="16">
+        <v>1</v>
+      </c>
+      <c r="J31" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="F32" s="16">
+        <v>8</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" s="16">
         <v>2</v>
       </c>
-      <c r="J31" s="19" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="F32" s="16">
-        <v>5</v>
-      </c>
-      <c r="G32" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="H32" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="I32" s="16">
-        <v>1</v>
-      </c>
       <c r="J32" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:15" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="14" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="F33" s="16">
         <v>8</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="I33" s="16">
         <v>2</v>
       </c>
       <c r="J33" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:15" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="14" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="C34" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="16" t="s">
         <v>99</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>122</v>
       </c>
       <c r="F34" s="16">
         <v>8</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="I34" s="16">
+        <v>3</v>
+      </c>
+      <c r="J34" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="F35" s="16">
+        <v>13</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="H35" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="I35" s="16">
         <v>2</v>
       </c>
-      <c r="J34" s="19" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="F35" s="16">
-        <v>8</v>
-      </c>
-      <c r="G35" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="H35" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="I35" s="16">
-        <v>3</v>
-      </c>
       <c r="J35" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="16" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="D36" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F36" s="16">
         <v>5</v>
       </c>
-      <c r="E36" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="F36" s="16">
-        <v>13</v>
-      </c>
       <c r="G36" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="I36" s="16">
         <v>2</v>
       </c>
       <c r="J36" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="16" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="F37" s="16">
         <v>5</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="I37" s="16">
+        <v>3</v>
+      </c>
+      <c r="J37" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="F38" s="16">
+        <v>8</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="I38" s="16">
         <v>2</v>
       </c>
-      <c r="J37" s="19" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="F38" s="16">
-        <v>5</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="H38" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="I38" s="16">
-        <v>3</v>
-      </c>
       <c r="J38" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="F39" s="16">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="I39" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J39" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="14" t="s">
-        <v>11</v>
+      <c r="C40" s="16" t="s">
+        <v>107</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="F40" s="16">
         <v>13</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="I40" s="16">
         <v>1</v>
       </c>
       <c r="J40" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="16" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>130</v>
+        <v>12</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="F41" s="16">
         <v>13</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="I41" s="16">
         <v>1</v>
       </c>
       <c r="J41" s="19" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="16" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="F42" s="16">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>151</v>
+        <v>109</v>
       </c>
       <c r="I42" s="16">
         <v>1</v>
       </c>
       <c r="J42" s="19" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="16" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="F43" s="16">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="I43" s="16">
         <v>1</v>
       </c>
       <c r="J43" s="19" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
@@ -6007,31 +6026,31 @@
     <row r="44" spans="1:15" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="16" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="F44" s="16">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H44" s="18" t="s">
-        <v>178</v>
+        <v>108</v>
       </c>
       <c r="I44" s="16">
         <v>1</v>
       </c>
       <c r="J44" s="19" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
@@ -6041,956 +6060,928 @@
     </row>
     <row r="45" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="16" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="F45" s="16">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H45" s="18" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="I45" s="16">
         <v>1</v>
       </c>
       <c r="J45" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="8"/>
     </row>
     <row r="46" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="16" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>35</v>
+        <v>134</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="F46" s="16">
         <v>8</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H46" s="18" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="I46" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J46" s="19" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="M46" s="2"/>
     </row>
     <row r="47" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="16" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>157</v>
+        <v>24</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="F47" s="16">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G47" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H47" s="18" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="I47" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J47" s="19" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="M47" s="1"/>
       <c r="N47" s="6"/>
     </row>
     <row r="48" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="16" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="F48" s="16">
         <v>5</v>
       </c>
       <c r="G48" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H48" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="I48" s="16">
         <v>1</v>
       </c>
       <c r="J48" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="M48" s="1"/>
       <c r="N48" s="7"/>
     </row>
     <row r="49" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="16" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="F49" s="16">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G49" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H49" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="I49" s="16">
         <v>1</v>
       </c>
       <c r="J49" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="M49" s="1"/>
       <c r="N49" s="8"/>
     </row>
     <row r="50" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="16" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E50" s="16" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="F50" s="16">
         <v>21</v>
       </c>
       <c r="G50" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H50" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="I50" s="16">
         <v>1</v>
       </c>
       <c r="J50" s="19" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="M50" s="2"/>
     </row>
     <row r="51" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="16" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="F51" s="16">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G51" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="I51" s="16">
         <v>1</v>
       </c>
       <c r="J51" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="6"/>
     </row>
     <row r="52" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="16" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="F52" s="16">
         <v>13</v>
       </c>
       <c r="G52" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H52" s="18" t="s">
-        <v>115</v>
+        <v>155</v>
       </c>
       <c r="I52" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J52" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="N52" s="7"/>
     </row>
     <row r="53" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="16" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="F53" s="16">
         <v>13</v>
       </c>
       <c r="G53" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H53" s="18" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="I53" s="16">
         <v>2</v>
       </c>
       <c r="J53" s="19" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="N53" s="8"/>
     </row>
     <row r="54" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="16" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>153</v>
+        <v>42</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="F54" s="16">
         <v>13</v>
       </c>
       <c r="G54" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H54" s="18" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="I54" s="16">
         <v>2</v>
       </c>
       <c r="J54" s="19" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="16" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="F55" s="16">
         <v>13</v>
       </c>
       <c r="G55" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H55" s="18" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="I55" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J55" s="19" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="N55" s="6"/>
     </row>
     <row r="56" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="16" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>69</v>
+        <v>136</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="F56" s="16">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G56" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H56" s="18" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="I56" s="16">
         <v>1</v>
       </c>
       <c r="J56" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="N56" s="7"/>
     </row>
     <row r="57" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="16" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="F57" s="16">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="G57" s="17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="H57" s="18" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="I57" s="16">
         <v>1</v>
       </c>
       <c r="J57" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="N57" s="8"/>
     </row>
     <row r="58" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="16" t="s">
-        <v>154</v>
+        <v>111</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="D58" s="15" t="s">
-        <v>79</v>
+        <v>137</v>
+      </c>
+      <c r="D58" s="16" t="s">
+        <v>3</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="F58" s="16">
         <v>21</v>
       </c>
       <c r="G58" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H58" s="18" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="I58" s="16">
         <v>1</v>
       </c>
       <c r="J58" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="N58" s="8"/>
     </row>
     <row r="59" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="16" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="F59" s="16">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="G59" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="H59" s="18" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="I59" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J59" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="16" t="s">
-        <v>135</v>
+        <v>7</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="F60" s="16">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G60" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="H60" s="18" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="I60" s="16">
         <v>2</v>
       </c>
       <c r="J60" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="N60" s="6"/>
     </row>
     <row r="61" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="16" t="s">
-        <v>10</v>
+        <v>113</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="D61" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F61" s="16">
         <v>5</v>
       </c>
-      <c r="E61" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="F61" s="16">
-        <v>13</v>
-      </c>
       <c r="G61" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="H61" s="18" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="I61" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J61" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="N61" s="7"/>
     </row>
     <row r="62" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="16" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="F62" s="16">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G62" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="H62" s="18" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="I62" s="16">
         <v>1</v>
       </c>
       <c r="J62" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="N62" s="8"/>
     </row>
     <row r="63" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="16" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="F63" s="16">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G63" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="H63" s="18" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="I63" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J63" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="16" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E64" s="16" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="F64" s="16">
         <v>13</v>
       </c>
       <c r="G64" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="H64" s="18" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="I64" s="16">
         <v>2</v>
       </c>
       <c r="J64" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="N64" s="6"/>
     </row>
     <row r="65" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="16" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E65" s="16" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="F65" s="16">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G65" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="H65" s="18" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="I65" s="16">
         <v>2</v>
       </c>
       <c r="J65" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="N65" s="7"/>
     </row>
     <row r="66" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="16" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E66" s="16" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="F66" s="16">
         <v>8</v>
       </c>
       <c r="G66" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="H66" s="18" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="I66" s="16">
         <v>2</v>
       </c>
       <c r="J66" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="N66" s="8"/>
     </row>
     <row r="67" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="16" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E67" s="16" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="F67" s="16">
         <v>8</v>
       </c>
       <c r="G67" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="H67" s="18" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="I67" s="16">
         <v>2</v>
       </c>
       <c r="J67" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
     </row>
     <row r="68" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="16" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E68" s="16" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="F68" s="16">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G68" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="H68" s="18" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="I68" s="16">
         <v>2</v>
       </c>
       <c r="J68" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
     </row>
     <row r="69" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="16" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="D69" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E69" s="16" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="F69" s="16">
         <v>13</v>
       </c>
       <c r="G69" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="H69" s="18" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="I69" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J69" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
     </row>
     <row r="70" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="16" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E70" s="16" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="F70" s="16">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G70" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="H70" s="18" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="I70" s="16">
         <v>1</v>
       </c>
       <c r="J70" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="16" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E71" s="16" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="F71" s="16">
         <v>21</v>
       </c>
       <c r="G71" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="H71" s="18" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="I71" s="16">
         <v>1</v>
       </c>
       <c r="J71" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="16" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="D72" s="16" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E72" s="16" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="F72" s="16">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G72" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="H72" s="18" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="I72" s="16">
         <v>1</v>
       </c>
       <c r="J72" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="16" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="D73" s="16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E73" s="16" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="F73" s="16">
         <v>13</v>
       </c>
       <c r="G73" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="H73" s="18" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="I73" s="16">
         <v>1</v>
       </c>
       <c r="J73" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="16" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E74" s="16" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="F74" s="16">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G74" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="H74" s="18" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="I74" s="16">
         <v>1</v>
       </c>
       <c r="J74" s="19" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
     </row>
     <row r="75" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="16" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E75" s="16" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="F75" s="16">
         <v>8</v>
       </c>
       <c r="G75" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="H75" s="18" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="I75" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J75" s="19" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="76" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C76" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="D76" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E76" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="F76" s="16">
-        <v>8</v>
-      </c>
-      <c r="G76" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="H76" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="I76" s="16">
-        <v>2</v>
-      </c>
-      <c r="J76" s="19" t="s">
-        <v>128</v>
-      </c>
-    </row>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="76" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="77" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7000,58 +6991,58 @@
     <mergeCell ref="B2:J2"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="D1 D3:D1048576 O44">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+  <conditionalFormatting sqref="D1 O44 D3:D1048576">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>"desejavel"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
       <formula>"Importante"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="18" operator="equal">
       <formula>"essencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
       <formula>"desejavel"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"Importante"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"essencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"desejavel"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"Importante"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"essencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"desejavel"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Importante"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"essencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:J3">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"desejavel"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Importante"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"essencial"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7089,48 +7080,48 @@
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
       <c r="I2" s="25" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="J2" s="25"/>
       <c r="K2" s="25"/>
       <c r="P2" s="25" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="Q2" s="25"/>
       <c r="R2" s="25"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="C3" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="D3" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="I3" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="J3" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="K3" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="P3" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="Q3" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="R3" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
@@ -7302,21 +7293,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD11765F9AC0004AAF0A4CAAFDFAF16A" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1cc742c03ab36aa87466a9c68feca297">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9fdc8751-6fef-42ec-b05c-835dd8c535b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c7a3de26cefa8042fb80bd6689b2d941" ns3:_="">
     <xsd:import namespace="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
@@ -7466,15 +7448,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B41A44-6A88-4A62-9CB5-74CD121A70D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8BD7424-A063-4080-9C1E-4A351D5C9788}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -7490,7 +7473,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30FF0F0A-C32A-40B6-8E34-61A738226646}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7506,4 +7489,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B41A44-6A88-4A62-9CB5-74CD121A70D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adicionar o backlog e documentação atualizados
</commit_message>
<xml_diff>
--- a/backlog-projeto-individual.xlsx
+++ b/backlog-projeto-individual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\OneDrive - SPTech School\PI\projeto\Gatices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5137C2FE-473F-49D9-BA06-B03780828670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F6BF58-65F5-40D7-B2B7-BCA374A2DC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{2AF606DE-C3BC-448B-8EBD-34B42A3F581A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="208">
   <si>
     <t xml:space="preserve">Requisito </t>
   </si>
@@ -631,6 +631,36 @@
   </si>
   <si>
     <t>Desenvolver algumas validações para os campos das telas de login e de cadastro, além de algumas mensagens de erro para orientar o usuário</t>
+  </si>
+  <si>
+    <t>Colocar o site e o banco de dados na VM</t>
+  </si>
+  <si>
+    <t>Configurar a máquina virtual para hospedagem do banco de dados e do site</t>
+  </si>
+  <si>
+    <t>Sprint03</t>
+  </si>
+  <si>
+    <t>Sprint04</t>
+  </si>
+  <si>
+    <t>Cadastrar os dados do gato no banco de dados</t>
+  </si>
+  <si>
+    <t>Persistir os dados do status do gato para utilizar na dashboard</t>
+  </si>
+  <si>
+    <t>Fazer os dados do gato aparecerem dinâmicamente na dashboard</t>
+  </si>
+  <si>
+    <t>Coletar os dados armazenados no banco de dados do gato e colocar na dashboard</t>
+  </si>
+  <si>
+    <t>Adicionar alguma forma do usuário poder enviar uma mensagem para o meu email</t>
+  </si>
+  <si>
+    <t>Por meio de uma biblioteca externa, fazer como que o usuário possa efetivamente enviar uma mensagem ao preencher os dados do formulário de fale conosco</t>
   </si>
 </sst>
 </file>
@@ -739,7 +769,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -919,12 +949,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
@@ -983,21 +1057,6 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1018,6 +1077,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4539,8 +4622,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2100501B-8E1F-4228-9C83-8B1543D6389D}" name="Tabela2" displayName="Tabela2" ref="B3:J84" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" tableBorderDxfId="28">
-  <autoFilter ref="B3:J84" xr:uid="{2100501B-8E1F-4228-9C83-8B1543D6389D}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2100501B-8E1F-4228-9C83-8B1543D6389D}" name="Tabela2" displayName="Tabela2" ref="B3:J87" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" tableBorderDxfId="28">
+  <autoFilter ref="B3:J87" xr:uid="{2100501B-8E1F-4228-9C83-8B1543D6389D}">
     <filterColumn colId="6">
       <filters>
         <filter val="Nicolas"/>
@@ -4918,10 +5001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC7B248-B611-44D6-BE4C-6F9175744526}">
-  <dimension ref="A1:N89"/>
+  <dimension ref="A1:N92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4939,17 +5022,17 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="22"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="33"/>
     </row>
     <row r="3" spans="2:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
@@ -5006,7 +5089,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -5064,7 +5147,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="2:10" s="5" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -6572,7 +6655,7 @@
         <v>1</v>
       </c>
       <c r="J57" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="N57" s="8"/>
     </row>
@@ -6602,7 +6685,7 @@
         <v>1</v>
       </c>
       <c r="J58" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="2:14" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -7195,25 +7278,25 @@
       </c>
     </row>
     <row r="79" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="25" t="s">
+      <c r="B79" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="C79" s="26" t="s">
+      <c r="C79" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="D79" s="26" t="s">
+      <c r="D79" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E79" s="26" t="s">
+      <c r="E79" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="F79" s="26">
+      <c r="F79" s="21">
         <v>13</v>
       </c>
-      <c r="G79" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="H79" s="24" t="s">
+      <c r="G79" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="H79" s="17" t="s">
         <v>100</v>
       </c>
       <c r="I79" s="14">
@@ -7224,25 +7307,25 @@
       </c>
     </row>
     <row r="80" spans="2:14" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="28" t="s">
+      <c r="B80" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="C80" s="29" t="s">
+      <c r="C80" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="D80" s="29" t="s">
+      <c r="D80" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E80" s="29" t="s">
+      <c r="E80" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="F80" s="29">
+      <c r="F80" s="24">
         <v>21</v>
       </c>
-      <c r="G80" s="29" t="s">
-        <v>185</v>
-      </c>
-      <c r="H80" s="24" t="s">
+      <c r="G80" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="H80" s="17" t="s">
         <v>100</v>
       </c>
       <c r="I80" s="14">
@@ -7253,105 +7336,210 @@
       </c>
     </row>
     <row r="81" spans="2:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="28" t="s">
+      <c r="B81" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="C81" s="28" t="s">
+      <c r="C81" s="23" t="s">
         <v>193</v>
       </c>
-      <c r="D81" s="28" t="s">
+      <c r="D81" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E81" s="28" t="s">
+      <c r="E81" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="F81" s="28">
+      <c r="F81" s="23">
         <v>21</v>
       </c>
-      <c r="G81" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="H81" s="24" t="s">
+      <c r="G81" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="H81" s="17" t="s">
         <v>100</v>
       </c>
       <c r="I81" s="14">
         <v>1</v>
       </c>
       <c r="J81" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="82" spans="2:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="28" t="s">
+      <c r="B82" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="C82" s="28" t="s">
+      <c r="C82" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="D82" s="28" t="s">
+      <c r="D82" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E82" s="28" t="s">
+      <c r="E82" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="F82" s="28">
+      <c r="F82" s="23">
         <v>21</v>
       </c>
-      <c r="G82" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="H82" s="24" t="s">
+      <c r="G82" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="H82" s="17" t="s">
         <v>100</v>
       </c>
       <c r="I82" s="14">
         <v>1</v>
       </c>
       <c r="J82" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="83" spans="2:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="28" t="s">
+      <c r="B83" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="C83" s="28" t="s">
+      <c r="C83" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="D83" s="28" t="s">
+      <c r="D83" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E83" s="28" t="s">
+      <c r="E83" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="F83" s="28">
+      <c r="F83" s="23">
         <v>21</v>
       </c>
-      <c r="G83" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="H83" s="28" t="s">
+      <c r="G83" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="H83" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="I83" s="30">
+      <c r="I83" s="25">
         <v>1</v>
       </c>
       <c r="J83" s="17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="84" spans="2:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="B84" s="24"/>
-      <c r="C84" s="24"/>
-      <c r="D84" s="24"/>
-      <c r="E84" s="24"/>
-      <c r="F84" s="24"/>
-      <c r="G84" s="24"/>
-      <c r="H84" s="24"/>
-      <c r="I84" s="14"/>
-      <c r="J84" s="17"/>
-    </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C89" s="31"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="84" spans="2:10" ht="36" x14ac:dyDescent="0.25">
+      <c r="B84" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="C84" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="D84" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E84" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="F84" s="27">
+        <v>13</v>
+      </c>
+      <c r="G84" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="H84" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="I84" s="14">
+        <v>1</v>
+      </c>
+      <c r="J84" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="85" spans="2:10" ht="36" x14ac:dyDescent="0.25">
+      <c r="B85" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C85" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="D85" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E85" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="F85" s="29">
+        <v>21</v>
+      </c>
+      <c r="G85" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="H85" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="I85" s="14">
+        <v>1</v>
+      </c>
+      <c r="J85" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="86" spans="2:10" ht="54" x14ac:dyDescent="0.25">
+      <c r="B86" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="C86" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="D86" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E86" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F86" s="24">
+        <v>21</v>
+      </c>
+      <c r="G86" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="H86" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="I86" s="14">
+        <v>1</v>
+      </c>
+      <c r="J86" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="87" spans="2:10" ht="54" x14ac:dyDescent="0.25">
+      <c r="B87" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="C87" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="D87" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E87" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="F87" s="29">
+        <v>13</v>
+      </c>
+      <c r="G87" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="H87" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="I87" s="14">
+        <v>1</v>
+      </c>
+      <c r="J87" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C92" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7446,21 +7634,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="I2" s="23" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="I2" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="P2" s="23" t="s">
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="P2" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -7660,6 +7848,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD11765F9AC0004AAF0A4CAAFDFAF16A" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1cc742c03ab36aa87466a9c68feca297">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9fdc8751-6fef-42ec-b05c-835dd8c535b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c7a3de26cefa8042fb80bd6689b2d941" ns3:_="">
     <xsd:import namespace="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
@@ -7809,12 +8003,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7825,6 +8013,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8BD7424-A063-4080-9C1E-4A351D5C9788}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30FF0F0A-C32A-40B6-8E34-61A738226646}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7842,22 +8046,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8BD7424-A063-4080-9C1E-4A351D5C9788}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B41A44-6A88-4A62-9CB5-74CD121A70D0}">
   <ds:schemaRefs>

</xml_diff>